<commit_message>
20250416 Low Carbon's done minus Optimize
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202504/Euronext World.xlsx
+++ b/GUI + Reviews/202504/Euronext World.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202504/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D935727F-CABA-45A0-8911-76C4B41EFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76B737E3-DFB0-47B1-9897-FF27CA291FAF}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{D935727F-CABA-45A0-8911-76C4B41EFCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD348EB-9613-4325-BA05-7017C82F1AAC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A565B4D7-AAB9-4ACB-84AE-66E5ED11F5EA}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{A565B4D7-AAB9-4ACB-84AE-66E5ED11F5EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13948,6 +13948,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F82E90EB-E3C4-4DA3-A67C-4CF06300E151}" name="Universe" displayName="Universe" ref="A1:K1500" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K1500" xr:uid="{F82E90EB-E3C4-4DA3-A67C-4CF06300E151}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{F30BE892-44C3-40C2-86C5-D8FB7EE6CE66}" name="Rank" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{17A554DC-104E-40DA-8C76-CF482D5E7080}" name="Ticker" dataDxfId="9"/>
@@ -14284,8 +14285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98404E7-87C0-43B4-9A85-B33B0FA6FBC2}">
   <dimension ref="A1:K1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1070" workbookViewId="0">
-      <selection activeCell="D1090" sqref="D1090"/>
+    <sheetView tabSelected="1" topLeftCell="A605" workbookViewId="0">
+      <selection activeCell="F624" sqref="F624"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22650,7 +22651,7 @@
         <v>20</v>
       </c>
       <c r="F239" s="1">
-        <v>381327700</v>
+        <v>381479460</v>
       </c>
       <c r="G239" s="1">
         <v>191.4873</v>
@@ -25135,7 +25136,7 @@
         <v>20</v>
       </c>
       <c r="F310" s="1">
-        <v>1272380200</v>
+        <v>1271093300</v>
       </c>
       <c r="G310" s="1">
         <v>93.677670000000006</v>
@@ -50825,7 +50826,7 @@
         <v>103</v>
       </c>
       <c r="F1044" s="1">
-        <v>217680560</v>
+        <v>216116100</v>
       </c>
       <c r="G1044" s="1">
         <v>37.375</v>
@@ -52435,10 +52436,10 @@
         <v>227</v>
       </c>
       <c r="F1090" s="1">
-        <v>11754106</v>
+        <v>117541060</v>
       </c>
       <c r="G1090" s="1">
-        <v>375.32420000000002</v>
+        <v>37.532420000000002</v>
       </c>
       <c r="H1090" s="1" t="s">
         <v>228</v>
@@ -58385,7 +58386,7 @@
         <v>32</v>
       </c>
       <c r="F1260" s="1">
-        <v>1082868300</v>
+        <v>1082967500</v>
       </c>
       <c r="G1260" s="1">
         <v>12.11585</v>
@@ -63110,7 +63111,7 @@
         <v>20</v>
       </c>
       <c r="F1395" s="1">
-        <v>609777900</v>
+        <v>604962900</v>
       </c>
       <c r="G1395" s="1">
         <v>234.86369999999999</v>

</xml_diff>